<commit_message>
Finished v6 draft, adde one lit resource, change W-L from loge to log10, deleted old versions of manuscript
</commit_message>
<xml_diff>
--- a/literature_resources/Summaries.xlsx
+++ b/literature_resources/Summaries.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="79">
   <si>
     <t>Age</t>
   </si>
@@ -343,6 +343,21 @@
   </si>
   <si>
     <t>Scales/Otos??</t>
+  </si>
+  <si>
+    <r>
+      <t>NL</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>*</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -744,8 +759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="D7" workbookViewId="0">
+      <selection activeCell="Q23" sqref="Q23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -824,7 +839,7 @@
         <v>3</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>4</v>
+        <v>78</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>58</v>
@@ -906,19 +921,19 @@
         <v>116</v>
       </c>
       <c r="G4" s="4">
-        <f>ROUND(IF(O4&lt;100,O4*1.0777,O4*1.0845),0)</f>
+        <f t="shared" ref="G4:H6" si="0">ROUND(IF(O4&lt;100,O4*1.0777,O4*1.0845),0)</f>
         <v>61</v>
       </c>
       <c r="H4" s="4">
-        <f>ROUND(IF(P4&lt;100,P4*1.0777,P4*1.0845),0)</f>
+        <f t="shared" si="0"/>
         <v>82</v>
       </c>
       <c r="I4" s="4">
-        <f t="shared" ref="I4:I9" si="0">ROUND(IF(Q4&lt;100,Q4*1.0777,Q4*1.0845),0)</f>
+        <f t="shared" ref="I4:I9" si="1">ROUND(IF(Q4&lt;100,Q4*1.0777,Q4*1.0845),0)</f>
         <v>87</v>
       </c>
       <c r="J4" s="4">
-        <f t="shared" ref="J4:J9" si="1">ROUND(IF(R4&lt;100,R4*1.0777,R4*1.0845),0)</f>
+        <f t="shared" ref="J4:J9" si="2">ROUND(IF(R4&lt;100,R4*1.0777,R4*1.0845),0)</f>
         <v>91</v>
       </c>
       <c r="K4" s="4" t="s">
@@ -928,7 +943,7 @@
         <v>9</v>
       </c>
       <c r="M4" s="4">
-        <f t="shared" ref="L4:M10" si="2">ROUND(IF(U4&lt;100,U4*1.0777,U4*1.0845),0)</f>
+        <f t="shared" ref="L4:M10" si="3">ROUND(IF(U4&lt;100,U4*1.0777,U4*1.0845),0)</f>
         <v>91</v>
       </c>
       <c r="O4" s="4">
@@ -996,31 +1011,31 @@
         <v>140</v>
       </c>
       <c r="G5" s="4">
-        <f>ROUND(IF(O5&lt;100,O5*1.0777,O5*1.0845),0)</f>
+        <f t="shared" si="0"/>
         <v>75</v>
       </c>
       <c r="H5" s="4">
-        <f>ROUND(IF(P5&lt;100,P5*1.0777,P5*1.0845),0)</f>
+        <f t="shared" si="0"/>
         <v>121</v>
       </c>
       <c r="I5" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>119</v>
       </c>
       <c r="J5" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>115</v>
       </c>
       <c r="K5" s="4">
-        <f t="shared" ref="K5:K10" si="3">ROUND(IF(S5&lt;100,S5*1.0777,S5*1.0845),0)</f>
+        <f t="shared" ref="K5:K10" si="4">ROUND(IF(S5&lt;100,S5*1.0777,S5*1.0845),0)</f>
         <v>127</v>
       </c>
       <c r="L5" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>118</v>
       </c>
       <c r="M5" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>114</v>
       </c>
       <c r="O5" s="4">
@@ -1088,31 +1103,31 @@
         <v>154</v>
       </c>
       <c r="G6" s="4">
-        <f>ROUND(IF(O6&lt;100,O6*1.0777,O6*1.0845),0)</f>
+        <f t="shared" si="0"/>
         <v>81</v>
       </c>
       <c r="H6" s="4">
-        <f>ROUND(IF(P6&lt;100,P6*1.0777,P6*1.0845),0)</f>
+        <f t="shared" si="0"/>
         <v>138</v>
       </c>
       <c r="I6" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>131</v>
       </c>
       <c r="J6" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>124</v>
       </c>
       <c r="K6" s="4">
+        <f t="shared" si="4"/>
+        <v>206</v>
+      </c>
+      <c r="L6" s="4">
         <f t="shared" si="3"/>
-        <v>206</v>
-      </c>
-      <c r="L6" s="4">
-        <f t="shared" si="2"/>
         <v>171</v>
       </c>
       <c r="M6" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>120</v>
       </c>
       <c r="O6" s="4">
@@ -1187,23 +1202,23 @@
         <v>150</v>
       </c>
       <c r="I7" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>138</v>
       </c>
       <c r="J7" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>130</v>
       </c>
       <c r="K7" s="4">
+        <f t="shared" si="4"/>
+        <v>238</v>
+      </c>
+      <c r="L7" s="4">
         <f t="shared" si="3"/>
-        <v>238</v>
-      </c>
-      <c r="L7" s="4">
-        <f t="shared" si="2"/>
         <v>210</v>
       </c>
       <c r="M7" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>128</v>
       </c>
       <c r="O7" s="4" t="s">
@@ -1278,23 +1293,23 @@
         <v>168</v>
       </c>
       <c r="I8" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>154</v>
       </c>
       <c r="J8" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>137</v>
       </c>
       <c r="K8" s="4">
+        <f t="shared" si="4"/>
+        <v>266</v>
+      </c>
+      <c r="L8" s="4">
         <f t="shared" si="3"/>
-        <v>266</v>
-      </c>
-      <c r="L8" s="4">
-        <f t="shared" si="2"/>
         <v>210</v>
       </c>
       <c r="M8" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>132</v>
       </c>
       <c r="O8" s="4" t="s">
@@ -1368,22 +1383,22 @@
         <v>9</v>
       </c>
       <c r="I9" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>169</v>
       </c>
       <c r="J9" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>147</v>
       </c>
       <c r="K9" s="4">
+        <f t="shared" si="4"/>
+        <v>269</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M9" s="4">
         <f t="shared" si="3"/>
-        <v>269</v>
-      </c>
-      <c r="L9" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="M9" s="4">
-        <f t="shared" si="2"/>
         <v>133</v>
       </c>
       <c r="O9" s="4" t="s">
@@ -1463,14 +1478,14 @@
         <v>9</v>
       </c>
       <c r="K10" s="4">
+        <f t="shared" si="4"/>
+        <v>279</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M10" s="4">
         <f t="shared" si="3"/>
-        <v>279</v>
-      </c>
-      <c r="L10" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="M10" s="4">
-        <f t="shared" si="2"/>
         <v>132</v>
       </c>
       <c r="O10" s="4" t="s">
@@ -1745,23 +1760,23 @@
         <v>55</v>
       </c>
       <c r="I14" s="4">
-        <f t="shared" ref="I14:I15" si="4">ROUND(IF(Q14&lt;100,Q14*1.0777,Q14*1.0845),0)</f>
+        <f t="shared" ref="I14:I15" si="5">ROUND(IF(Q14&lt;100,Q14*1.0777,Q14*1.0845),0)</f>
         <v>89</v>
       </c>
       <c r="J14" s="4">
-        <f t="shared" ref="J14:J15" si="5">ROUND(IF(R14&lt;100,R14*1.0777,R14*1.0845),0)</f>
+        <f t="shared" ref="J14:J15" si="6">ROUND(IF(R14&lt;100,R14*1.0777,R14*1.0845),0)</f>
         <v>84</v>
       </c>
       <c r="K14" s="4">
-        <f t="shared" ref="K14:K15" si="6">ROUND(IF(S14&lt;100,S14*1.0777,S14*1.0845),0)</f>
+        <f t="shared" ref="K14:K15" si="7">ROUND(IF(S14&lt;100,S14*1.0777,S14*1.0845),0)</f>
         <v>114</v>
       </c>
       <c r="L14" s="4">
-        <f t="shared" ref="L14:M15" si="7">ROUND(IF(T14&lt;100,T14*1.0777,T14*1.0845),0)</f>
+        <f t="shared" ref="L14:M15" si="8">ROUND(IF(T14&lt;100,T14*1.0777,T14*1.0845),0)</f>
         <v>114</v>
       </c>
       <c r="M14" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>29</v>
       </c>
       <c r="O14" s="4">
@@ -1817,23 +1832,23 @@
         <v>168</v>
       </c>
       <c r="I15" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>171</v>
       </c>
       <c r="J15" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>150</v>
       </c>
       <c r="K15" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>298</v>
       </c>
       <c r="L15" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>211</v>
       </c>
       <c r="M15" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>233</v>
       </c>
       <c r="O15" s="5">
@@ -1941,7 +1956,7 @@
         <v>3</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>4</v>
+        <v>78</v>
       </c>
       <c r="I19" s="3" t="s">
         <v>58</v>
@@ -1997,19 +2012,19 @@
         <v>117</v>
       </c>
       <c r="G20" s="4">
-        <f t="shared" ref="G20:G22" si="8">ROUND(IF(O20&lt;100,O20*1.0777,O20*1.0845),0)</f>
+        <f t="shared" ref="G20:G22" si="9">ROUND(IF(O20&lt;100,O20*1.0777,O20*1.0845),0)</f>
         <v>61</v>
       </c>
       <c r="H20" s="4">
-        <f t="shared" ref="H20:H22" si="9">ROUND(IF(P20&lt;100,P20*1.0777,P20*1.0845),0)</f>
+        <f t="shared" ref="H20:H22" si="10">ROUND(IF(P20&lt;100,P20*1.0777,P20*1.0845),0)</f>
         <v>83</v>
       </c>
       <c r="I20" s="4">
-        <f t="shared" ref="I20:I24" si="10">ROUND(IF(Q20&lt;100,Q20*1.0777,Q20*1.0845),0)</f>
+        <f t="shared" ref="I20:I24" si="11">ROUND(IF(Q20&lt;100,Q20*1.0777,Q20*1.0845),0)</f>
         <v>99</v>
       </c>
       <c r="J20" s="4">
-        <f t="shared" ref="J20:J22" si="11">ROUND(IF(R20&lt;100,R20*1.0777,R20*1.0845),0)</f>
+        <f t="shared" ref="J20:J22" si="12">ROUND(IF(R20&lt;100,R20*1.0777,R20*1.0845),0)</f>
         <v>88</v>
       </c>
       <c r="K20" s="7" t="s">
@@ -2019,7 +2034,7 @@
         <v>9</v>
       </c>
       <c r="M20" s="4">
-        <f t="shared" ref="M20:M23" si="12">ROUND(IF(U20&lt;100,U20*1.0777,U20*1.0845),0)</f>
+        <f t="shared" ref="M20:M23" si="13">ROUND(IF(U20&lt;100,U20*1.0777,U20*1.0845),0)</f>
         <v>79</v>
       </c>
       <c r="O20" s="7">
@@ -2063,31 +2078,31 @@
         <v>128</v>
       </c>
       <c r="G21" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>69</v>
       </c>
       <c r="H21" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>118</v>
       </c>
       <c r="I21" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>123</v>
       </c>
       <c r="J21" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>97</v>
       </c>
       <c r="K21" s="4">
-        <f t="shared" ref="K21:K25" si="13">ROUND(IF(S21&lt;100,S21*1.0777,S21*1.0845),0)</f>
+        <f t="shared" ref="K21:K25" si="14">ROUND(IF(S21&lt;100,S21*1.0777,S21*1.0845),0)</f>
         <v>131</v>
       </c>
       <c r="L21" s="4">
-        <f t="shared" ref="L21:L23" si="14">ROUND(IF(T21&lt;100,T21*1.0777,T21*1.0845),0)</f>
+        <f t="shared" ref="L21:L23" si="15">ROUND(IF(T21&lt;100,T21*1.0777,T21*1.0845),0)</f>
         <v>120</v>
       </c>
       <c r="M21" s="4">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>101</v>
       </c>
       <c r="O21" s="7">
@@ -2131,31 +2146,31 @@
         <v>140</v>
       </c>
       <c r="G22" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>77</v>
       </c>
       <c r="H22" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>128</v>
       </c>
       <c r="I22" s="4">
-        <f t="shared" si="10"/>
-        <v>123</v>
+        <f t="shared" si="11"/>
+        <v>126</v>
       </c>
       <c r="J22" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>117</v>
       </c>
       <c r="K22" s="4">
+        <f t="shared" si="14"/>
+        <v>208</v>
+      </c>
+      <c r="L22" s="4">
+        <f t="shared" si="15"/>
+        <v>166</v>
+      </c>
+      <c r="M22" s="4">
         <f t="shared" si="13"/>
-        <v>208</v>
-      </c>
-      <c r="L22" s="4">
-        <f t="shared" si="14"/>
-        <v>166</v>
-      </c>
-      <c r="M22" s="4">
-        <f t="shared" si="12"/>
         <v>110</v>
       </c>
       <c r="O22" s="7">
@@ -2165,7 +2180,7 @@
         <v>118</v>
       </c>
       <c r="Q22" s="7">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="R22" s="7">
         <v>108</v>
@@ -2206,22 +2221,22 @@
         <v>144</v>
       </c>
       <c r="I23" s="4">
-        <f t="shared" si="10"/>
-        <v>123</v>
+        <f t="shared" si="11"/>
+        <v>126</v>
       </c>
       <c r="J23" s="7" t="s">
         <v>9</v>
       </c>
       <c r="K23" s="4">
+        <f t="shared" si="14"/>
+        <v>228</v>
+      </c>
+      <c r="L23" s="4">
+        <f t="shared" si="15"/>
+        <v>193</v>
+      </c>
+      <c r="M23" s="4">
         <f t="shared" si="13"/>
-        <v>228</v>
-      </c>
-      <c r="L23" s="4">
-        <f t="shared" si="14"/>
-        <v>193</v>
-      </c>
-      <c r="M23" s="4">
-        <f t="shared" si="12"/>
         <v>114</v>
       </c>
       <c r="O23" s="7" t="s">
@@ -2231,7 +2246,7 @@
         <v>133</v>
       </c>
       <c r="Q23" s="7">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="R23" s="7" t="s">
         <v>9</v>
@@ -2271,14 +2286,14 @@
         <v>9</v>
       </c>
       <c r="I24" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>132</v>
       </c>
       <c r="J24" s="7" t="s">
         <v>9</v>
       </c>
       <c r="K24" s="4">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>201</v>
       </c>
       <c r="L24" s="7" t="s">
@@ -2340,7 +2355,7 @@
         <v>9</v>
       </c>
       <c r="K25" s="4">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>244</v>
       </c>
       <c r="L25" s="7" t="s">
@@ -2600,23 +2615,23 @@
         <v>55</v>
       </c>
       <c r="I30" s="4">
-        <f t="shared" ref="I30:I31" si="15">ROUND(IF(Q30&lt;100,Q30*1.0777,Q30*1.0845),0)</f>
+        <f t="shared" ref="I30:I31" si="16">ROUND(IF(Q30&lt;100,Q30*1.0777,Q30*1.0845),0)</f>
         <v>95</v>
       </c>
       <c r="J30" s="4">
-        <f t="shared" ref="J30:J31" si="16">ROUND(IF(R30&lt;100,R30*1.0777,R30*1.0845),0)</f>
+        <f t="shared" ref="J30:J31" si="17">ROUND(IF(R30&lt;100,R30*1.0777,R30*1.0845),0)</f>
         <v>84</v>
       </c>
       <c r="K30" s="4">
-        <f t="shared" ref="K30:K31" si="17">ROUND(IF(S30&lt;100,S30*1.0777,S30*1.0845),0)</f>
+        <f t="shared" ref="K30:K31" si="18">ROUND(IF(S30&lt;100,S30*1.0777,S30*1.0845),0)</f>
         <v>114</v>
       </c>
       <c r="L30" s="4">
-        <f t="shared" ref="L30:M31" si="18">ROUND(IF(T30&lt;100,T30*1.0777,T30*1.0845),0)</f>
+        <f t="shared" ref="L30:M31" si="19">ROUND(IF(T30&lt;100,T30*1.0777,T30*1.0845),0)</f>
         <v>114</v>
       </c>
       <c r="M30" s="4">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>67</v>
       </c>
       <c r="O30" s="4">
@@ -2664,23 +2679,23 @@
         <v>153</v>
       </c>
       <c r="I31" s="4">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>139</v>
       </c>
       <c r="J31" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>123</v>
       </c>
       <c r="K31" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>255</v>
       </c>
       <c r="L31" s="4">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>190</v>
       </c>
       <c r="M31" s="4">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>132</v>
       </c>
       <c r="O31" s="5">

</xml_diff>

<commit_message>
Fixed growth script relative to other studies.
</commit_message>
<xml_diff>
--- a/literature_resources/Summaries.xlsx
+++ b/literature_resources/Summaries.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="80">
   <si>
     <t>Age</t>
   </si>
@@ -358,6 +358,9 @@
       </rPr>
       <t>*</t>
     </r>
+  </si>
+  <si>
+    <t>Table 5</t>
   </si>
 </sst>
 </file>
@@ -759,8 +762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D7" workbookViewId="0">
-      <selection activeCell="Q23" sqref="Q23"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="AB8" sqref="AB8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -1168,7 +1171,7 @@
         <v>38</v>
       </c>
       <c r="AB6" t="s">
-        <v>41</v>
+        <v>79</v>
       </c>
       <c r="AC6" s="1" t="s">
         <v>44</v>

</xml_diff>